<commit_message>
disabled pdf option, and minor changes to template
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_50_rpt_PF_NetRecoverySummaryByQuarter.xlsx
+++ b/backend/reports/xlsx/Tab_50_rpt_PF_NetRecoverySummaryByQuarter.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarmich\source\repos\gdx-agreements-tracker\backend\reports\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E9EC59-9ECB-1149-8C0C-687A8EB0C6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BDBD89-BBAF-4073-B805-DBEFF8332F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$2:$2</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -77,9 +80,6 @@
     <t>Net Recoveries</t>
   </si>
   <si>
-    <t>{$r.total_recoveries}</t>
-  </si>
-  <si>
     <t>{$r.less_all_project_expenses}</t>
   </si>
   <si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Portfolios</t>
+  </si>
+  <si>
+    <t>{$r.total_recoveries_portfolio}</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -346,13 +349,13 @@
     <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -434,9 +437,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -474,7 +477,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -580,7 +583,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -722,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -733,44 +736,45 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.19921875" customWidth="1"/>
+    <col min="2" max="2" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="16" t="s">
-        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -806,45 +810,45 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
@@ -860,78 +864,78 @@
       <c r="K4" s="6"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="L5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="10" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;Lrpt_PF_NetRecoverySummaryByQuarter&amp;C&amp;P of &amp;N&amp;R{$date}</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add portfolios to Tab 50 header
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_50_rpt_PF_NetRecoverySummaryByQuarter.xlsx
+++ b/backend/reports/xlsx/Tab_50_rpt_PF_NetRecoverySummaryByQuarter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anlashle/Repos/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE18479-86EB-EC46-AE57-CB8D9FEE8160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE550B5-4568-0E4D-AEC8-C7BC4EB791EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="7380" windowWidth="34560" windowHeight="20060" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>{$r1.portfolio_name}</t>
   </si>
@@ -164,19 +164,14 @@
     <t>Portfolios</t>
   </si>
   <si>
-    <t>Net Recovery Summary By Quarter for Fiscal Year {$fy}</t>
-  </si>
-  <si>
-    <t>{#abr=d.portAbbrev[i]}</t>
-  </si>
-  <si>
-    <t>{$abr.abbr}</t>
-  </si>
-  <si>
-    <t>{#abr1=d.portAbbrev[i+1]}</t>
-  </si>
-  <si>
-    <t>{$abr1.abbr}</t>
+    <t>{#abr=d.portAbbrev}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Recovery Summary By Quarter for Fiscal Year {$fy}
+</t>
+  </si>
+  <si>
+    <t>Fiscal Year: {$fy}; Portfolio: {$abr};</t>
   </si>
 </sst>
 </file>
@@ -186,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -222,6 +217,11 @@
       <sz val="8.5"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -243,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -280,72 +280,55 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
+      <left/>
       <right style="medium">
         <color rgb="FFBFBFBF"/>
       </right>
       <top style="medium">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FFBFBFBF"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FFBFBFBF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
       <right style="medium">
         <color rgb="FFBFBFBF"/>
       </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
@@ -358,13 +341,29 @@
     <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -400,8 +399,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>32837</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2411054</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>680356</xdr:rowOff>
     </xdr:to>
@@ -742,18 +741,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F20F7FF-D6FB-0145-BC76-92F810195548}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
@@ -764,200 +763,202 @@
     <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="17" thickBot="1">
-      <c r="A2" s="14" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1">
+      <c r="A1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" s="19" customFormat="1" ht="22" customHeight="1">
+      <c r="A2" s="18"/>
+      <c r="B2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="A3" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L3" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="17" thickBot="1">
-      <c r="A3" s="12" t="s">
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="17" thickBot="1">
+      <c r="A4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L4" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="17" thickBot="1">
-      <c r="A4" s="13" t="s">
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="17" thickBot="1">
+      <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="17" thickBot="1">
-      <c r="A5" s="11" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L6" s="8" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="C15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>